<commit_message>
Places page css fixed
</commit_message>
<xml_diff>
--- a/backend/data/data.xlsx
+++ b/backend/data/data.xlsx
@@ -1165,16 +1165,16 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2186,8 +2186,8 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1"/>
@@ -2197,8 +2197,8 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1"/>
@@ -2208,8 +2208,8 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1"/>
@@ -2219,8 +2219,8 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1"/>
@@ -2230,8 +2230,8 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1"/>
@@ -2241,8 +2241,8 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1"/>
@@ -2252,41 +2252,41 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="10"/>
+      <c r="D31" s="9"/>
       <c r="E31" s="1"/>
       <c r="F31" s="3"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="10"/>
+      <c r="D32" s="9"/>
       <c r="E32" s="1"/>
       <c r="F32" s="3"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="10"/>
+      <c r="D33" s="9"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3"/>
@@ -2296,74 +2296,74 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="10"/>
+      <c r="D35" s="9"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="3"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="10"/>
+      <c r="D36" s="9"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="3"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="10"/>
+      <c r="D37" s="9"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="3"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="10"/>
+      <c r="D38" s="9"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="3"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="10"/>
+      <c r="D39" s="9"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="3"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="10"/>
+      <c r="D40" s="9"/>
       <c r="E40" s="1"/>
       <c r="F40" s="3"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2405,7 +2405,7 @@
     <col min="22" max="22" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2457,7 +2457,7 @@
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2497,7 +2497,7 @@
       <c r="M2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="3">
         <v>200</v>
       </c>
       <c r="O2" s="2"/>
@@ -2509,7 +2509,7 @@
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2549,7 +2549,7 @@
       <c r="M3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="3">
         <v>200</v>
       </c>
       <c r="O3" s="2"/>
@@ -2561,7 +2561,7 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2601,7 +2601,7 @@
       <c r="M4" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="3">
         <v>200</v>
       </c>
       <c r="O4" s="2"/>
@@ -2613,7 +2613,7 @@
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2653,7 +2653,7 @@
       <c r="M5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="3">
         <v>200</v>
       </c>
       <c r="O5" s="2"/>
@@ -2665,7 +2665,7 @@
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2705,7 +2705,7 @@
       <c r="M6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="3">
         <v>200</v>
       </c>
       <c r="O6" s="2"/>
@@ -2717,7 +2717,7 @@
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2757,7 +2757,7 @@
       <c r="M7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="3">
         <v>200</v>
       </c>
       <c r="O7" s="2"/>
@@ -2769,7 +2769,7 @@
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2809,7 +2809,7 @@
       <c r="M8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="3">
         <v>200</v>
       </c>
       <c r="O8" s="2"/>
@@ -2821,7 +2821,7 @@
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2861,7 +2861,7 @@
       <c r="M9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="3">
         <v>200</v>
       </c>
       <c r="O9" s="2"/>
@@ -2873,7 +2873,7 @@
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2913,7 +2913,7 @@
       <c r="M10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="3">
         <v>200</v>
       </c>
       <c r="O10" s="2"/>
@@ -2925,7 +2925,7 @@
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2965,7 +2965,7 @@
       <c r="M11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="3">
         <v>200</v>
       </c>
       <c r="O11" s="2"/>
@@ -2977,7 +2977,7 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="M12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="3">
         <v>200</v>
       </c>
       <c r="O12" s="2"/>
@@ -3029,7 +3029,7 @@
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="M13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="3">
         <v>200</v>
       </c>
       <c r="O13" s="2"/>
@@ -3081,7 +3081,7 @@
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3121,7 +3121,7 @@
       <c r="M14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="3">
         <v>200</v>
       </c>
       <c r="O14" s="2"/>
@@ -3133,7 +3133,7 @@
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3173,7 +3173,7 @@
       <c r="M15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="3">
         <v>200</v>
       </c>
       <c r="O15" s="2"/>
@@ -3185,7 +3185,7 @@
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3225,7 +3225,7 @@
       <c r="M16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="3">
         <v>200</v>
       </c>
       <c r="O16" s="2"/>
@@ -3237,7 +3237,7 @@
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3277,7 +3277,7 @@
       <c r="M17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17" s="3">
         <v>200</v>
       </c>
       <c r="O17" s="2"/>
@@ -3289,7 +3289,7 @@
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3329,7 +3329,7 @@
       <c r="M18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="3">
         <v>200</v>
       </c>
       <c r="O18" s="2"/>
@@ -3341,7 +3341,7 @@
       <c r="U18" s="8"/>
       <c r="V18" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3381,7 +3381,7 @@
       <c r="M19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19" s="3">
         <v>200</v>
       </c>
       <c r="O19" s="2"/>
@@ -3393,7 +3393,7 @@
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3433,7 +3433,7 @@
       <c r="M20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N20" s="3">
         <v>200</v>
       </c>
       <c r="O20" s="2"/>
@@ -3445,7 +3445,7 @@
       <c r="U20" s="8"/>
       <c r="V20" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3485,7 +3485,7 @@
       <c r="M21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N21" s="9">
+      <c r="N21" s="3">
         <v>200</v>
       </c>
       <c r="O21" s="2"/>
@@ -3497,7 +3497,7 @@
       <c r="U21" s="8"/>
       <c r="V21" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3537,7 +3537,7 @@
       <c r="M22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N22" s="3">
         <v>200</v>
       </c>
       <c r="O22" s="2"/>
@@ -3549,7 +3549,7 @@
       <c r="U22" s="8"/>
       <c r="V22" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3589,7 +3589,7 @@
       <c r="M23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="9">
+      <c r="N23" s="3">
         <v>200</v>
       </c>
       <c r="O23" s="2"/>
@@ -3601,7 +3601,7 @@
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3641,7 +3641,7 @@
       <c r="M24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N24" s="9">
+      <c r="N24" s="3">
         <v>200</v>
       </c>
       <c r="O24" s="2"/>
@@ -3653,7 +3653,7 @@
       <c r="U24" s="8"/>
       <c r="V24" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3693,7 +3693,7 @@
       <c r="M25" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N25" s="9">
+      <c r="N25" s="3">
         <v>200</v>
       </c>
       <c r="O25" s="2"/>
@@ -3705,7 +3705,7 @@
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3745,7 +3745,7 @@
       <c r="M26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N26" s="9">
+      <c r="N26" s="3">
         <v>200</v>
       </c>
       <c r="O26" s="2"/>
@@ -3757,7 +3757,7 @@
       <c r="U26" s="8"/>
       <c r="V26" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3797,7 +3797,7 @@
       <c r="M27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N27" s="9">
+      <c r="N27" s="3">
         <v>200</v>
       </c>
       <c r="O27" s="2"/>
@@ -3849,7 +3849,7 @@
       <c r="M28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N28" s="9">
+      <c r="N28" s="3">
         <v>200</v>
       </c>
       <c r="O28" s="2"/>
@@ -3901,7 +3901,7 @@
       <c r="M29" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N29" s="9">
+      <c r="N29" s="3">
         <v>200</v>
       </c>
       <c r="O29" s="2"/>
@@ -3953,7 +3953,7 @@
       <c r="M30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N30" s="9">
+      <c r="N30" s="3">
         <v>200</v>
       </c>
       <c r="O30" s="2"/>
@@ -4005,7 +4005,7 @@
       <c r="M31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N31" s="9">
+      <c r="N31" s="3">
         <v>200</v>
       </c>
       <c r="O31" s="2"/>
@@ -4057,7 +4057,7 @@
       <c r="M32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N32" s="9">
+      <c r="N32" s="3">
         <v>200</v>
       </c>
       <c r="O32" s="2"/>
@@ -4109,7 +4109,7 @@
       <c r="M33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N33" s="9">
+      <c r="N33" s="3">
         <v>200</v>
       </c>
       <c r="O33" s="2"/>
@@ -4161,7 +4161,7 @@
       <c r="M34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N34" s="9">
+      <c r="N34" s="3">
         <v>200</v>
       </c>
       <c r="O34" s="2"/>
@@ -4213,7 +4213,7 @@
       <c r="M35" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N35" s="9">
+      <c r="N35" s="3">
         <v>200</v>
       </c>
       <c r="O35" s="2"/>
@@ -4265,7 +4265,7 @@
       <c r="M36" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N36" s="9">
+      <c r="N36" s="3">
         <v>200</v>
       </c>
       <c r="O36" s="2"/>
@@ -4317,7 +4317,7 @@
       <c r="M37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N37" s="9">
+      <c r="N37" s="3">
         <v>200</v>
       </c>
       <c r="O37" s="2"/>
@@ -4369,7 +4369,7 @@
       <c r="M38" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N38" s="9">
+      <c r="N38" s="3">
         <v>200</v>
       </c>
       <c r="O38" s="2"/>
@@ -4421,7 +4421,7 @@
       <c r="M39" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N39" s="9">
+      <c r="N39" s="3">
         <v>200</v>
       </c>
       <c r="O39" s="2"/>
@@ -4473,7 +4473,7 @@
       <c r="M40" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N40" s="9">
+      <c r="N40" s="3">
         <v>200</v>
       </c>
       <c r="O40" s="2"/>
@@ -4525,7 +4525,7 @@
       <c r="M41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N41" s="9">
+      <c r="N41" s="3">
         <v>200</v>
       </c>
       <c r="O41" s="2"/>
@@ -4577,7 +4577,7 @@
       <c r="M42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N42" s="9">
+      <c r="N42" s="3">
         <v>200</v>
       </c>
       <c r="O42" s="2"/>
@@ -4629,7 +4629,7 @@
       <c r="M43" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N43" s="9">
+      <c r="N43" s="3">
         <v>200</v>
       </c>
       <c r="O43" s="2"/>
@@ -4681,7 +4681,7 @@
       <c r="M44" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N44" s="9">
+      <c r="N44" s="3">
         <v>200</v>
       </c>
       <c r="O44" s="2"/>
@@ -4733,7 +4733,7 @@
       <c r="M45" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N45" s="9">
+      <c r="N45" s="3">
         <v>200</v>
       </c>
       <c r="O45" s="2"/>
@@ -4785,7 +4785,7 @@
       <c r="M46" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N46" s="9">
+      <c r="N46" s="3">
         <v>200</v>
       </c>
       <c r="O46" s="2"/>
@@ -4837,7 +4837,7 @@
       <c r="M47" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N47" s="9">
+      <c r="N47" s="3">
         <v>200</v>
       </c>
       <c r="O47" s="2"/>
@@ -4889,7 +4889,7 @@
       <c r="M48" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N48" s="9">
+      <c r="N48" s="3">
         <v>200</v>
       </c>
       <c r="O48" s="2"/>
@@ -4941,7 +4941,7 @@
       <c r="M49" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N49" s="9">
+      <c r="N49" s="3">
         <v>200</v>
       </c>
       <c r="O49" s="2"/>
@@ -4993,7 +4993,7 @@
       <c r="M50" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N50" s="9">
+      <c r="N50" s="3">
         <v>200</v>
       </c>
       <c r="O50" s="2"/>
@@ -5045,7 +5045,7 @@
       <c r="M51" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N51" s="9">
+      <c r="N51" s="3">
         <v>200</v>
       </c>
       <c r="O51" s="2"/>
@@ -5097,7 +5097,7 @@
       <c r="M52" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N52" s="9">
+      <c r="N52" s="3">
         <v>200</v>
       </c>
       <c r="O52" s="2"/>
@@ -5149,7 +5149,7 @@
       <c r="M53" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N53" s="9">
+      <c r="N53" s="3">
         <v>200</v>
       </c>
       <c r="O53" s="2"/>
@@ -5201,7 +5201,7 @@
       <c r="M54" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N54" s="9">
+      <c r="N54" s="3">
         <v>200</v>
       </c>
       <c r="O54" s="2"/>
@@ -5253,7 +5253,7 @@
       <c r="M55" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N55" s="9">
+      <c r="N55" s="3">
         <v>200</v>
       </c>
       <c r="O55" s="2"/>
@@ -5305,7 +5305,7 @@
       <c r="M56" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N56" s="9">
+      <c r="N56" s="3">
         <v>200</v>
       </c>
       <c r="O56" s="2"/>
@@ -5357,7 +5357,7 @@
       <c r="M57" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N57" s="9">
+      <c r="N57" s="3">
         <v>200</v>
       </c>
       <c r="O57" s="2"/>
@@ -5409,7 +5409,7 @@
       <c r="M58" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N58" s="9">
+      <c r="N58" s="3">
         <v>200</v>
       </c>
       <c r="O58" s="2"/>
@@ -5461,7 +5461,7 @@
       <c r="M59" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N59" s="9">
+      <c r="N59" s="3">
         <v>200</v>
       </c>
       <c r="O59" s="2"/>
@@ -5513,7 +5513,7 @@
       <c r="M60" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N60" s="9">
+      <c r="N60" s="3">
         <v>200</v>
       </c>
       <c r="O60" s="2"/>
@@ -5565,7 +5565,7 @@
       <c r="M61" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N61" s="9">
+      <c r="N61" s="3">
         <v>200</v>
       </c>
       <c r="O61" s="2"/>
@@ -5617,7 +5617,7 @@
       <c r="M62" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N62" s="9">
+      <c r="N62" s="3">
         <v>200</v>
       </c>
       <c r="O62" s="2"/>
@@ -5669,7 +5669,7 @@
       <c r="M63" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N63" s="9">
+      <c r="N63" s="3">
         <v>200</v>
       </c>
       <c r="O63" s="2"/>
@@ -5721,7 +5721,7 @@
       <c r="M64" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N64" s="9">
+      <c r="N64" s="3">
         <v>200</v>
       </c>
       <c r="O64" s="2"/>
@@ -5773,7 +5773,7 @@
       <c r="M65" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N65" s="9">
+      <c r="N65" s="3">
         <v>200</v>
       </c>
       <c r="O65" s="2"/>
@@ -5825,7 +5825,7 @@
       <c r="M66" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N66" s="9">
+      <c r="N66" s="3">
         <v>200</v>
       </c>
       <c r="O66" s="2"/>
@@ -5877,7 +5877,7 @@
       <c r="M67" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N67" s="9">
+      <c r="N67" s="3">
         <v>200</v>
       </c>
       <c r="O67" s="2"/>
@@ -5929,7 +5929,7 @@
       <c r="M68" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N68" s="9">
+      <c r="N68" s="3">
         <v>200</v>
       </c>
       <c r="O68" s="2"/>
@@ -5981,7 +5981,7 @@
       <c r="M69" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N69" s="9">
+      <c r="N69" s="3">
         <v>200</v>
       </c>
       <c r="O69" s="2"/>
@@ -6033,7 +6033,7 @@
       <c r="M70" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N70" s="9">
+      <c r="N70" s="3">
         <v>200</v>
       </c>
       <c r="O70" s="2"/>
@@ -6085,7 +6085,7 @@
       <c r="M71" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N71" s="9">
+      <c r="N71" s="3">
         <v>200</v>
       </c>
       <c r="O71" s="2"/>
@@ -6137,7 +6137,7 @@
       <c r="M72" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N72" s="9">
+      <c r="N72" s="3">
         <v>200</v>
       </c>
       <c r="O72" s="2"/>
@@ -6189,7 +6189,7 @@
       <c r="M73" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N73" s="9">
+      <c r="N73" s="3">
         <v>200</v>
       </c>
       <c r="O73" s="2"/>
@@ -6241,7 +6241,7 @@
       <c r="M74" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N74" s="9">
+      <c r="N74" s="3">
         <v>200</v>
       </c>
       <c r="O74" s="2"/>
@@ -6293,7 +6293,7 @@
       <c r="M75" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N75" s="9">
+      <c r="N75" s="3">
         <v>200</v>
       </c>
       <c r="O75" s="2"/>
@@ -6345,7 +6345,7 @@
       <c r="M76" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="N76" s="9">
+      <c r="N76" s="3">
         <v>200</v>
       </c>
       <c r="O76" s="2"/>
@@ -6397,7 +6397,7 @@
       <c r="M77" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="N77" s="9">
+      <c r="N77" s="3">
         <v>200</v>
       </c>
       <c r="O77" s="2"/>
@@ -6418,12 +6418,12 @@
       <c r="F78" s="2"/>
       <c r="G78" s="8"/>
       <c r="H78" s="6"/>
-      <c r="I78" s="10"/>
+      <c r="I78" s="9"/>
       <c r="J78" s="1"/>
       <c r="K78" s="8"/>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
-      <c r="N78" s="7"/>
+      <c r="N78" s="10"/>
       <c r="O78" s="2"/>
       <c r="P78" s="8"/>
       <c r="Q78" s="2"/>
@@ -6447,7 +6447,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
-      <c r="N79" s="7"/>
+      <c r="N79" s="10"/>
       <c r="O79" s="2"/>
       <c r="P79" s="8"/>
       <c r="Q79" s="2"/>
@@ -6466,12 +6466,12 @@
       <c r="F80" s="2"/>
       <c r="G80" s="8"/>
       <c r="H80" s="6"/>
-      <c r="I80" s="10"/>
+      <c r="I80" s="9"/>
       <c r="J80" s="1"/>
       <c r="K80" s="8"/>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
-      <c r="N80" s="7"/>
+      <c r="N80" s="10"/>
       <c r="O80" s="2"/>
       <c r="P80" s="8"/>
       <c r="Q80" s="2"/>
@@ -6490,12 +6490,12 @@
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
       <c r="H81" s="6"/>
-      <c r="I81" s="10"/>
+      <c r="I81" s="9"/>
       <c r="J81" s="1"/>
       <c r="K81" s="8"/>
       <c r="L81" s="3"/>
       <c r="M81" s="1"/>
-      <c r="N81" s="7"/>
+      <c r="N81" s="10"/>
       <c r="O81" s="2"/>
       <c r="P81" s="8"/>
       <c r="Q81" s="2"/>
@@ -6519,7 +6519,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
-      <c r="N82" s="7"/>
+      <c r="N82" s="10"/>
       <c r="O82" s="2"/>
       <c r="P82" s="8"/>
       <c r="Q82" s="2"/>
@@ -6543,7 +6543,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
-      <c r="N83" s="7"/>
+      <c r="N83" s="10"/>
       <c r="O83" s="2"/>
       <c r="P83" s="8"/>
       <c r="Q83" s="2"/>
@@ -6562,12 +6562,12 @@
       <c r="F84" s="2"/>
       <c r="G84" s="8"/>
       <c r="H84" s="6"/>
-      <c r="I84" s="10"/>
+      <c r="I84" s="9"/>
       <c r="J84" s="1"/>
       <c r="K84" s="8"/>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
-      <c r="N84" s="7"/>
+      <c r="N84" s="10"/>
       <c r="O84" s="2"/>
       <c r="P84" s="8"/>
       <c r="Q84" s="2"/>
@@ -6591,7 +6591,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
-      <c r="N85" s="7"/>
+      <c r="N85" s="10"/>
       <c r="O85" s="2"/>
       <c r="P85" s="8"/>
       <c r="Q85" s="2"/>
@@ -6615,7 +6615,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
-      <c r="N86" s="7"/>
+      <c r="N86" s="10"/>
       <c r="O86" s="2"/>
       <c r="P86" s="8"/>
       <c r="Q86" s="2"/>
@@ -6639,7 +6639,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
-      <c r="N87" s="7"/>
+      <c r="N87" s="10"/>
       <c r="O87" s="2"/>
       <c r="P87" s="8"/>
       <c r="Q87" s="2"/>
@@ -6663,7 +6663,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
-      <c r="N88" s="7"/>
+      <c r="N88" s="10"/>
       <c r="O88" s="2"/>
       <c r="P88" s="8"/>
       <c r="Q88" s="2"/>
@@ -6687,7 +6687,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
-      <c r="N89" s="7"/>
+      <c r="N89" s="10"/>
       <c r="O89" s="2"/>
       <c r="P89" s="8"/>
       <c r="Q89" s="2"/>
@@ -6711,7 +6711,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
-      <c r="N90" s="7"/>
+      <c r="N90" s="10"/>
       <c r="O90" s="2"/>
       <c r="P90" s="8"/>
       <c r="Q90" s="2"/>
@@ -6730,12 +6730,12 @@
       <c r="F91" s="8"/>
       <c r="G91" s="2"/>
       <c r="H91" s="6"/>
-      <c r="I91" s="10"/>
+      <c r="I91" s="9"/>
       <c r="J91" s="1"/>
       <c r="K91" s="8"/>
       <c r="L91" s="3"/>
       <c r="M91" s="1"/>
-      <c r="N91" s="7"/>
+      <c r="N91" s="10"/>
       <c r="O91" s="2"/>
       <c r="P91" s="8"/>
       <c r="Q91" s="2"/>
@@ -6754,12 +6754,12 @@
       <c r="F92" s="8"/>
       <c r="G92" s="8"/>
       <c r="H92" s="6"/>
-      <c r="I92" s="10"/>
+      <c r="I92" s="9"/>
       <c r="J92" s="1"/>
       <c r="K92" s="8"/>
       <c r="L92" s="3"/>
       <c r="M92" s="1"/>
-      <c r="N92" s="7"/>
+      <c r="N92" s="10"/>
       <c r="O92" s="2"/>
       <c r="P92" s="8"/>
       <c r="Q92" s="2"/>
@@ -6778,12 +6778,12 @@
       <c r="F93" s="8"/>
       <c r="G93" s="8"/>
       <c r="H93" s="6"/>
-      <c r="I93" s="10"/>
+      <c r="I93" s="9"/>
       <c r="J93" s="1"/>
       <c r="K93" s="8"/>
       <c r="L93" s="3"/>
       <c r="M93" s="1"/>
-      <c r="N93" s="7"/>
+      <c r="N93" s="10"/>
       <c r="O93" s="2"/>
       <c r="P93" s="8"/>
       <c r="Q93" s="2"/>
@@ -6802,12 +6802,12 @@
       <c r="F94" s="8"/>
       <c r="G94" s="8"/>
       <c r="H94" s="6"/>
-      <c r="I94" s="10"/>
+      <c r="I94" s="9"/>
       <c r="J94" s="1"/>
       <c r="K94" s="8"/>
       <c r="L94" s="3"/>
       <c r="M94" s="1"/>
-      <c r="N94" s="7"/>
+      <c r="N94" s="10"/>
       <c r="O94" s="2"/>
       <c r="P94" s="8"/>
       <c r="Q94" s="2"/>
@@ -6826,12 +6826,12 @@
       <c r="F95" s="8"/>
       <c r="G95" s="8"/>
       <c r="H95" s="6"/>
-      <c r="I95" s="10"/>
+      <c r="I95" s="9"/>
       <c r="J95" s="1"/>
       <c r="K95" s="8"/>
       <c r="L95" s="3"/>
       <c r="M95" s="1"/>
-      <c r="N95" s="7"/>
+      <c r="N95" s="10"/>
       <c r="O95" s="2"/>
       <c r="P95" s="8"/>
       <c r="Q95" s="2"/>
@@ -6850,12 +6850,12 @@
       <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="6"/>
-      <c r="I96" s="10"/>
+      <c r="I96" s="9"/>
       <c r="J96" s="1"/>
       <c r="K96" s="8"/>
       <c r="L96" s="3"/>
       <c r="M96" s="1"/>
-      <c r="N96" s="7"/>
+      <c r="N96" s="10"/>
       <c r="O96" s="2"/>
       <c r="P96" s="8"/>
       <c r="Q96" s="2"/>
@@ -6874,12 +6874,12 @@
       <c r="F97" s="8"/>
       <c r="G97" s="8"/>
       <c r="H97" s="6"/>
-      <c r="I97" s="10"/>
+      <c r="I97" s="9"/>
       <c r="J97" s="1"/>
       <c r="K97" s="8"/>
       <c r="L97" s="3"/>
       <c r="M97" s="1"/>
-      <c r="N97" s="7"/>
+      <c r="N97" s="10"/>
       <c r="O97" s="2"/>
       <c r="P97" s="8"/>
       <c r="Q97" s="2"/>
@@ -6898,12 +6898,12 @@
       <c r="F98" s="8"/>
       <c r="G98" s="8"/>
       <c r="H98" s="6"/>
-      <c r="I98" s="10"/>
+      <c r="I98" s="9"/>
       <c r="J98" s="1"/>
       <c r="K98" s="8"/>
       <c r="L98" s="3"/>
       <c r="M98" s="1"/>
-      <c r="N98" s="7"/>
+      <c r="N98" s="10"/>
       <c r="O98" s="2"/>
       <c r="P98" s="8"/>
       <c r="Q98" s="2"/>
@@ -6922,12 +6922,12 @@
       <c r="F99" s="8"/>
       <c r="G99" s="8"/>
       <c r="H99" s="6"/>
-      <c r="I99" s="10"/>
+      <c r="I99" s="9"/>
       <c r="J99" s="1"/>
       <c r="K99" s="8"/>
       <c r="L99" s="3"/>
       <c r="M99" s="1"/>
-      <c r="N99" s="7"/>
+      <c r="N99" s="10"/>
       <c r="O99" s="2"/>
       <c r="P99" s="8"/>
       <c r="Q99" s="2"/>
@@ -6946,12 +6946,12 @@
       <c r="F100" s="8"/>
       <c r="G100" s="8"/>
       <c r="H100" s="6"/>
-      <c r="I100" s="10"/>
+      <c r="I100" s="9"/>
       <c r="J100" s="1"/>
       <c r="K100" s="8"/>
       <c r="L100" s="3"/>
       <c r="M100" s="1"/>
-      <c r="N100" s="7"/>
+      <c r="N100" s="10"/>
       <c r="O100" s="2"/>
       <c r="P100" s="8"/>
       <c r="Q100" s="2"/>
@@ -6970,12 +6970,12 @@
       <c r="F101" s="8"/>
       <c r="G101" s="8"/>
       <c r="H101" s="6"/>
-      <c r="I101" s="10"/>
+      <c r="I101" s="9"/>
       <c r="J101" s="1"/>
       <c r="K101" s="8"/>
       <c r="L101" s="3"/>
       <c r="M101" s="1"/>
-      <c r="N101" s="7"/>
+      <c r="N101" s="10"/>
       <c r="O101" s="2"/>
       <c r="P101" s="8"/>
       <c r="Q101" s="2"/>
@@ -6994,12 +6994,12 @@
       <c r="F102" s="8"/>
       <c r="G102" s="8"/>
       <c r="H102" s="6"/>
-      <c r="I102" s="10"/>
+      <c r="I102" s="9"/>
       <c r="J102" s="1"/>
       <c r="K102" s="8"/>
       <c r="L102" s="3"/>
       <c r="M102" s="1"/>
-      <c r="N102" s="7"/>
+      <c r="N102" s="10"/>
       <c r="O102" s="2"/>
       <c r="P102" s="8"/>
       <c r="Q102" s="2"/>
@@ -7018,12 +7018,12 @@
       <c r="F103" s="8"/>
       <c r="G103" s="8"/>
       <c r="H103" s="6"/>
-      <c r="I103" s="10"/>
+      <c r="I103" s="9"/>
       <c r="J103" s="1"/>
       <c r="K103" s="8"/>
       <c r="L103" s="3"/>
       <c r="M103" s="1"/>
-      <c r="N103" s="7"/>
+      <c r="N103" s="10"/>
       <c r="O103" s="2"/>
       <c r="P103" s="8"/>
       <c r="Q103" s="2"/>
@@ -7042,12 +7042,12 @@
       <c r="F104" s="8"/>
       <c r="G104" s="8"/>
       <c r="H104" s="6"/>
-      <c r="I104" s="10"/>
+      <c r="I104" s="9"/>
       <c r="J104" s="1"/>
       <c r="K104" s="8"/>
       <c r="L104" s="3"/>
       <c r="M104" s="1"/>
-      <c r="N104" s="7"/>
+      <c r="N104" s="10"/>
       <c r="O104" s="2"/>
       <c r="P104" s="8"/>
       <c r="Q104" s="2"/>
@@ -7066,12 +7066,12 @@
       <c r="F105" s="8"/>
       <c r="G105" s="8"/>
       <c r="H105" s="6"/>
-      <c r="I105" s="10"/>
+      <c r="I105" s="9"/>
       <c r="J105" s="1"/>
       <c r="K105" s="8"/>
       <c r="L105" s="3"/>
       <c r="M105" s="1"/>
-      <c r="N105" s="7"/>
+      <c r="N105" s="10"/>
       <c r="O105" s="2"/>
       <c r="P105" s="8"/>
       <c r="Q105" s="2"/>
@@ -7090,12 +7090,12 @@
       <c r="F106" s="8"/>
       <c r="G106" s="8"/>
       <c r="H106" s="6"/>
-      <c r="I106" s="10"/>
+      <c r="I106" s="9"/>
       <c r="J106" s="1"/>
       <c r="K106" s="8"/>
       <c r="L106" s="3"/>
       <c r="M106" s="1"/>
-      <c r="N106" s="7"/>
+      <c r="N106" s="10"/>
       <c r="O106" s="2"/>
       <c r="P106" s="8"/>
       <c r="Q106" s="2"/>
@@ -7114,12 +7114,12 @@
       <c r="F107" s="8"/>
       <c r="G107" s="8"/>
       <c r="H107" s="6"/>
-      <c r="I107" s="10"/>
+      <c r="I107" s="9"/>
       <c r="J107" s="1"/>
       <c r="K107" s="8"/>
       <c r="L107" s="3"/>
       <c r="M107" s="1"/>
-      <c r="N107" s="7"/>
+      <c r="N107" s="10"/>
       <c r="O107" s="2"/>
       <c r="P107" s="8"/>
       <c r="Q107" s="2"/>
@@ -7138,12 +7138,12 @@
       <c r="F108" s="8"/>
       <c r="G108" s="8"/>
       <c r="H108" s="6"/>
-      <c r="I108" s="10"/>
+      <c r="I108" s="9"/>
       <c r="J108" s="1"/>
       <c r="K108" s="8"/>
       <c r="L108" s="3"/>
       <c r="M108" s="1"/>
-      <c r="N108" s="7"/>
+      <c r="N108" s="10"/>
       <c r="O108" s="2"/>
       <c r="P108" s="8"/>
       <c r="Q108" s="2"/>
@@ -7162,12 +7162,12 @@
       <c r="F109" s="8"/>
       <c r="G109" s="8"/>
       <c r="H109" s="6"/>
-      <c r="I109" s="10"/>
+      <c r="I109" s="9"/>
       <c r="J109" s="1"/>
       <c r="K109" s="8"/>
       <c r="L109" s="3"/>
       <c r="M109" s="1"/>
-      <c r="N109" s="7"/>
+      <c r="N109" s="10"/>
       <c r="O109" s="2"/>
       <c r="P109" s="8"/>
       <c r="Q109" s="2"/>
@@ -7186,12 +7186,12 @@
       <c r="F110" s="8"/>
       <c r="G110" s="8"/>
       <c r="H110" s="6"/>
-      <c r="I110" s="10"/>
+      <c r="I110" s="9"/>
       <c r="J110" s="1"/>
       <c r="K110" s="8"/>
       <c r="L110" s="3"/>
       <c r="M110" s="1"/>
-      <c r="N110" s="7"/>
+      <c r="N110" s="10"/>
       <c r="O110" s="2"/>
       <c r="P110" s="8"/>
       <c r="Q110" s="2"/>
@@ -7210,12 +7210,12 @@
       <c r="F111" s="8"/>
       <c r="G111" s="8"/>
       <c r="H111" s="6"/>
-      <c r="I111" s="10"/>
+      <c r="I111" s="9"/>
       <c r="J111" s="1"/>
       <c r="K111" s="8"/>
       <c r="L111" s="3"/>
       <c r="M111" s="1"/>
-      <c r="N111" s="7"/>
+      <c r="N111" s="10"/>
       <c r="O111" s="2"/>
       <c r="P111" s="8"/>
       <c r="Q111" s="2"/>
@@ -7234,12 +7234,12 @@
       <c r="F112" s="8"/>
       <c r="G112" s="8"/>
       <c r="H112" s="6"/>
-      <c r="I112" s="10"/>
+      <c r="I112" s="9"/>
       <c r="J112" s="1"/>
       <c r="K112" s="8"/>
       <c r="L112" s="3"/>
       <c r="M112" s="1"/>
-      <c r="N112" s="7"/>
+      <c r="N112" s="10"/>
       <c r="O112" s="2"/>
       <c r="P112" s="8"/>
       <c r="Q112" s="2"/>
@@ -7258,12 +7258,12 @@
       <c r="F113" s="8"/>
       <c r="G113" s="8"/>
       <c r="H113" s="6"/>
-      <c r="I113" s="10"/>
+      <c r="I113" s="9"/>
       <c r="J113" s="1"/>
       <c r="K113" s="8"/>
       <c r="L113" s="3"/>
       <c r="M113" s="1"/>
-      <c r="N113" s="7"/>
+      <c r="N113" s="10"/>
       <c r="O113" s="2"/>
       <c r="P113" s="8"/>
       <c r="Q113" s="2"/>
@@ -7282,12 +7282,12 @@
       <c r="F114" s="8"/>
       <c r="G114" s="8"/>
       <c r="H114" s="6"/>
-      <c r="I114" s="10"/>
+      <c r="I114" s="9"/>
       <c r="J114" s="1"/>
       <c r="K114" s="8"/>
       <c r="L114" s="3"/>
       <c r="M114" s="1"/>
-      <c r="N114" s="7"/>
+      <c r="N114" s="10"/>
       <c r="O114" s="2"/>
       <c r="P114" s="8"/>
       <c r="Q114" s="2"/>
@@ -7498,12 +7498,12 @@
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
       <c r="H123" s="1"/>
-      <c r="I123" s="10"/>
+      <c r="I123" s="9"/>
       <c r="J123" s="1"/>
       <c r="K123" s="8"/>
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
-      <c r="N123" s="7"/>
+      <c r="N123" s="10"/>
       <c r="O123" s="1"/>
       <c r="P123" s="8"/>
       <c r="Q123" s="1"/>
@@ -7522,12 +7522,12 @@
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
       <c r="H124" s="1"/>
-      <c r="I124" s="10"/>
+      <c r="I124" s="9"/>
       <c r="J124" s="1"/>
       <c r="K124" s="8"/>
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
-      <c r="N124" s="7"/>
+      <c r="N124" s="10"/>
       <c r="O124" s="1"/>
       <c r="P124" s="8"/>
       <c r="Q124" s="1"/>
@@ -7546,12 +7546,12 @@
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
       <c r="H125" s="1"/>
-      <c r="I125" s="10"/>
+      <c r="I125" s="9"/>
       <c r="J125" s="1"/>
       <c r="K125" s="8"/>
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
-      <c r="N125" s="7"/>
+      <c r="N125" s="10"/>
       <c r="O125" s="1"/>
       <c r="P125" s="8"/>
       <c r="Q125" s="1"/>
@@ -7570,12 +7570,12 @@
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
       <c r="H126" s="1"/>
-      <c r="I126" s="10"/>
+      <c r="I126" s="9"/>
       <c r="J126" s="1"/>
       <c r="K126" s="8"/>
       <c r="L126" s="1"/>
       <c r="M126" s="1"/>
-      <c r="N126" s="7"/>
+      <c r="N126" s="10"/>
       <c r="O126" s="1"/>
       <c r="P126" s="8"/>
       <c r="Q126" s="1"/>
@@ -7594,12 +7594,12 @@
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
       <c r="H127" s="1"/>
-      <c r="I127" s="10"/>
+      <c r="I127" s="9"/>
       <c r="J127" s="1"/>
       <c r="K127" s="8"/>
       <c r="L127" s="1"/>
       <c r="M127" s="1"/>
-      <c r="N127" s="7"/>
+      <c r="N127" s="10"/>
       <c r="O127" s="1"/>
       <c r="P127" s="8"/>
       <c r="Q127" s="1"/>
@@ -7618,12 +7618,12 @@
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
       <c r="H128" s="1"/>
-      <c r="I128" s="10"/>
+      <c r="I128" s="9"/>
       <c r="J128" s="1"/>
       <c r="K128" s="8"/>
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
-      <c r="N128" s="7"/>
+      <c r="N128" s="10"/>
       <c r="O128" s="1"/>
       <c r="P128" s="8"/>
       <c r="Q128" s="1"/>
@@ -7642,12 +7642,12 @@
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
       <c r="H129" s="1"/>
-      <c r="I129" s="10"/>
+      <c r="I129" s="9"/>
       <c r="J129" s="1"/>
       <c r="K129" s="8"/>
       <c r="L129" s="1"/>
       <c r="M129" s="1"/>
-      <c r="N129" s="7"/>
+      <c r="N129" s="10"/>
       <c r="O129" s="1"/>
       <c r="P129" s="8"/>
       <c r="Q129" s="1"/>
@@ -7666,12 +7666,12 @@
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
       <c r="H130" s="1"/>
-      <c r="I130" s="10"/>
+      <c r="I130" s="9"/>
       <c r="J130" s="1"/>
       <c r="K130" s="8"/>
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
-      <c r="N130" s="7"/>
+      <c r="N130" s="10"/>
       <c r="O130" s="1"/>
       <c r="P130" s="8"/>
       <c r="Q130" s="1"/>
@@ -7690,12 +7690,12 @@
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
       <c r="H131" s="1"/>
-      <c r="I131" s="10"/>
+      <c r="I131" s="9"/>
       <c r="J131" s="1"/>
       <c r="K131" s="8"/>
       <c r="L131" s="1"/>
       <c r="M131" s="1"/>
-      <c r="N131" s="7"/>
+      <c r="N131" s="10"/>
       <c r="O131" s="1"/>
       <c r="P131" s="8"/>
       <c r="Q131" s="1"/>
@@ -7714,12 +7714,12 @@
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
       <c r="H132" s="1"/>
-      <c r="I132" s="10"/>
+      <c r="I132" s="9"/>
       <c r="J132" s="1"/>
       <c r="K132" s="8"/>
       <c r="L132" s="1"/>
       <c r="M132" s="1"/>
-      <c r="N132" s="7"/>
+      <c r="N132" s="10"/>
       <c r="O132" s="1"/>
       <c r="P132" s="8"/>
       <c r="Q132" s="1"/>
@@ -7738,12 +7738,12 @@
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
       <c r="H133" s="1"/>
-      <c r="I133" s="10"/>
+      <c r="I133" s="9"/>
       <c r="J133" s="1"/>
       <c r="K133" s="8"/>
       <c r="L133" s="1"/>
       <c r="M133" s="1"/>
-      <c r="N133" s="7"/>
+      <c r="N133" s="10"/>
       <c r="O133" s="1"/>
       <c r="P133" s="8"/>
       <c r="Q133" s="1"/>
@@ -7762,12 +7762,12 @@
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
       <c r="H134" s="1"/>
-      <c r="I134" s="10"/>
+      <c r="I134" s="9"/>
       <c r="J134" s="1"/>
       <c r="K134" s="8"/>
       <c r="L134" s="1"/>
       <c r="M134" s="1"/>
-      <c r="N134" s="7"/>
+      <c r="N134" s="10"/>
       <c r="O134" s="1"/>
       <c r="P134" s="8"/>
       <c r="Q134" s="1"/>
@@ -7786,12 +7786,12 @@
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
       <c r="H135" s="1"/>
-      <c r="I135" s="10"/>
+      <c r="I135" s="9"/>
       <c r="J135" s="1"/>
       <c r="K135" s="8"/>
       <c r="L135" s="1"/>
       <c r="M135" s="1"/>
-      <c r="N135" s="7"/>
+      <c r="N135" s="10"/>
       <c r="O135" s="1"/>
       <c r="P135" s="8"/>
       <c r="Q135" s="1"/>
@@ -7810,12 +7810,12 @@
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
       <c r="H136" s="1"/>
-      <c r="I136" s="10"/>
+      <c r="I136" s="9"/>
       <c r="J136" s="1"/>
       <c r="K136" s="8"/>
       <c r="L136" s="1"/>
       <c r="M136" s="1"/>
-      <c r="N136" s="7"/>
+      <c r="N136" s="10"/>
       <c r="O136" s="1"/>
       <c r="P136" s="8"/>
       <c r="Q136" s="1"/>
@@ -7834,12 +7834,12 @@
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
       <c r="H137" s="1"/>
-      <c r="I137" s="10"/>
+      <c r="I137" s="9"/>
       <c r="J137" s="1"/>
       <c r="K137" s="8"/>
       <c r="L137" s="1"/>
       <c r="M137" s="1"/>
-      <c r="N137" s="7"/>
+      <c r="N137" s="10"/>
       <c r="O137" s="1"/>
       <c r="P137" s="8"/>
       <c r="Q137" s="1"/>
@@ -7858,12 +7858,12 @@
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
       <c r="H138" s="1"/>
-      <c r="I138" s="10"/>
+      <c r="I138" s="9"/>
       <c r="J138" s="1"/>
       <c r="K138" s="8"/>
       <c r="L138" s="1"/>
       <c r="M138" s="1"/>
-      <c r="N138" s="7"/>
+      <c r="N138" s="10"/>
       <c r="O138" s="1"/>
       <c r="P138" s="8"/>
       <c r="Q138" s="1"/>
@@ -7882,12 +7882,12 @@
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
       <c r="H139" s="1"/>
-      <c r="I139" s="10"/>
+      <c r="I139" s="9"/>
       <c r="J139" s="1"/>
       <c r="K139" s="8"/>
       <c r="L139" s="1"/>
       <c r="M139" s="1"/>
-      <c r="N139" s="7"/>
+      <c r="N139" s="10"/>
       <c r="O139" s="1"/>
       <c r="P139" s="8"/>
       <c r="Q139" s="1"/>
@@ -7906,12 +7906,12 @@
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
       <c r="H140" s="1"/>
-      <c r="I140" s="10"/>
+      <c r="I140" s="9"/>
       <c r="J140" s="1"/>
       <c r="K140" s="8"/>
       <c r="L140" s="1"/>
       <c r="M140" s="1"/>
-      <c r="N140" s="7"/>
+      <c r="N140" s="10"/>
       <c r="O140" s="1"/>
       <c r="P140" s="8"/>
       <c r="Q140" s="1"/>
@@ -7930,12 +7930,12 @@
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
       <c r="H141" s="1"/>
-      <c r="I141" s="10"/>
+      <c r="I141" s="9"/>
       <c r="J141" s="1"/>
       <c r="K141" s="8"/>
       <c r="L141" s="1"/>
       <c r="M141" s="1"/>
-      <c r="N141" s="7"/>
+      <c r="N141" s="10"/>
       <c r="O141" s="1"/>
       <c r="P141" s="8"/>
       <c r="Q141" s="1"/>
@@ -7954,12 +7954,12 @@
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
       <c r="H142" s="1"/>
-      <c r="I142" s="10"/>
+      <c r="I142" s="9"/>
       <c r="J142" s="1"/>
       <c r="K142" s="8"/>
       <c r="L142" s="1"/>
       <c r="M142" s="1"/>
-      <c r="N142" s="7"/>
+      <c r="N142" s="10"/>
       <c r="O142" s="1"/>
       <c r="P142" s="8"/>
       <c r="Q142" s="1"/>
@@ -7978,12 +7978,12 @@
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
       <c r="H143" s="1"/>
-      <c r="I143" s="10"/>
+      <c r="I143" s="9"/>
       <c r="J143" s="1"/>
       <c r="K143" s="8"/>
       <c r="L143" s="1"/>
       <c r="M143" s="1"/>
-      <c r="N143" s="7"/>
+      <c r="N143" s="10"/>
       <c r="O143" s="1"/>
       <c r="P143" s="8"/>
       <c r="Q143" s="1"/>
@@ -8002,12 +8002,12 @@
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
       <c r="H144" s="1"/>
-      <c r="I144" s="10"/>
+      <c r="I144" s="9"/>
       <c r="J144" s="1"/>
       <c r="K144" s="8"/>
       <c r="L144" s="1"/>
       <c r="M144" s="1"/>
-      <c r="N144" s="7"/>
+      <c r="N144" s="10"/>
       <c r="O144" s="1"/>
       <c r="P144" s="8"/>
       <c r="Q144" s="1"/>
@@ -8026,12 +8026,12 @@
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
       <c r="H145" s="1"/>
-      <c r="I145" s="10"/>
+      <c r="I145" s="9"/>
       <c r="J145" s="1"/>
       <c r="K145" s="8"/>
       <c r="L145" s="1"/>
       <c r="M145" s="1"/>
-      <c r="N145" s="7"/>
+      <c r="N145" s="10"/>
       <c r="O145" s="1"/>
       <c r="P145" s="8"/>
       <c r="Q145" s="1"/>
@@ -8050,12 +8050,12 @@
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
       <c r="H146" s="1"/>
-      <c r="I146" s="10"/>
+      <c r="I146" s="9"/>
       <c r="J146" s="1"/>
       <c r="K146" s="8"/>
       <c r="L146" s="1"/>
       <c r="M146" s="1"/>
-      <c r="N146" s="7"/>
+      <c r="N146" s="10"/>
       <c r="O146" s="1"/>
       <c r="P146" s="8"/>
       <c r="Q146" s="1"/>
@@ -8074,12 +8074,12 @@
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
       <c r="H147" s="1"/>
-      <c r="I147" s="10"/>
+      <c r="I147" s="9"/>
       <c r="J147" s="1"/>
       <c r="K147" s="8"/>
       <c r="L147" s="1"/>
       <c r="M147" s="1"/>
-      <c r="N147" s="7"/>
+      <c r="N147" s="10"/>
       <c r="O147" s="1"/>
       <c r="P147" s="8"/>
       <c r="Q147" s="1"/>
@@ -8098,12 +8098,12 @@
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
       <c r="H148" s="1"/>
-      <c r="I148" s="10"/>
+      <c r="I148" s="9"/>
       <c r="J148" s="1"/>
       <c r="K148" s="8"/>
       <c r="L148" s="1"/>
       <c r="M148" s="1"/>
-      <c r="N148" s="7"/>
+      <c r="N148" s="10"/>
       <c r="O148" s="1"/>
       <c r="P148" s="8"/>
       <c r="Q148" s="1"/>
@@ -8122,12 +8122,12 @@
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
       <c r="H149" s="1"/>
-      <c r="I149" s="10"/>
+      <c r="I149" s="9"/>
       <c r="J149" s="1"/>
       <c r="K149" s="8"/>
       <c r="L149" s="1"/>
       <c r="M149" s="1"/>
-      <c r="N149" s="7"/>
+      <c r="N149" s="10"/>
       <c r="O149" s="1"/>
       <c r="P149" s="8"/>
       <c r="Q149" s="1"/>
@@ -8146,12 +8146,12 @@
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
       <c r="H150" s="1"/>
-      <c r="I150" s="10"/>
+      <c r="I150" s="9"/>
       <c r="J150" s="1"/>
       <c r="K150" s="8"/>
       <c r="L150" s="1"/>
       <c r="M150" s="1"/>
-      <c r="N150" s="7"/>
+      <c r="N150" s="10"/>
       <c r="O150" s="1"/>
       <c r="P150" s="8"/>
       <c r="Q150" s="1"/>
@@ -8170,12 +8170,12 @@
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
       <c r="H151" s="1"/>
-      <c r="I151" s="10"/>
+      <c r="I151" s="9"/>
       <c r="J151" s="1"/>
       <c r="K151" s="8"/>
       <c r="L151" s="1"/>
       <c r="M151" s="1"/>
-      <c r="N151" s="7"/>
+      <c r="N151" s="10"/>
       <c r="O151" s="1"/>
       <c r="P151" s="8"/>
       <c r="Q151" s="1"/>
@@ -8194,12 +8194,12 @@
       <c r="F152" s="2"/>
       <c r="G152" s="2"/>
       <c r="H152" s="1"/>
-      <c r="I152" s="10"/>
+      <c r="I152" s="9"/>
       <c r="J152" s="1"/>
       <c r="K152" s="8"/>
       <c r="L152" s="1"/>
       <c r="M152" s="1"/>
-      <c r="N152" s="7"/>
+      <c r="N152" s="10"/>
       <c r="O152" s="1"/>
       <c r="P152" s="8"/>
       <c r="Q152" s="1"/>
@@ -8218,12 +8218,12 @@
       <c r="F153" s="2"/>
       <c r="G153" s="2"/>
       <c r="H153" s="1"/>
-      <c r="I153" s="10"/>
+      <c r="I153" s="9"/>
       <c r="J153" s="1"/>
       <c r="K153" s="8"/>
       <c r="L153" s="1"/>
       <c r="M153" s="1"/>
-      <c r="N153" s="7"/>
+      <c r="N153" s="10"/>
       <c r="O153" s="1"/>
       <c r="P153" s="8"/>
       <c r="Q153" s="1"/>
@@ -8242,12 +8242,12 @@
       <c r="F154" s="2"/>
       <c r="G154" s="2"/>
       <c r="H154" s="1"/>
-      <c r="I154" s="10"/>
+      <c r="I154" s="9"/>
       <c r="J154" s="1"/>
       <c r="K154" s="8"/>
       <c r="L154" s="1"/>
       <c r="M154" s="1"/>
-      <c r="N154" s="7"/>
+      <c r="N154" s="10"/>
       <c r="O154" s="1"/>
       <c r="P154" s="8"/>
       <c r="Q154" s="1"/>
@@ -8266,12 +8266,12 @@
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
       <c r="H155" s="1"/>
-      <c r="I155" s="10"/>
+      <c r="I155" s="9"/>
       <c r="J155" s="1"/>
       <c r="K155" s="8"/>
       <c r="L155" s="1"/>
       <c r="M155" s="1"/>
-      <c r="N155" s="7"/>
+      <c r="N155" s="10"/>
       <c r="O155" s="1"/>
       <c r="P155" s="8"/>
       <c r="Q155" s="1"/>
@@ -8290,12 +8290,12 @@
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
       <c r="H156" s="1"/>
-      <c r="I156" s="10"/>
+      <c r="I156" s="9"/>
       <c r="J156" s="1"/>
       <c r="K156" s="8"/>
       <c r="L156" s="1"/>
       <c r="M156" s="1"/>
-      <c r="N156" s="7"/>
+      <c r="N156" s="10"/>
       <c r="O156" s="1"/>
       <c r="P156" s="8"/>
       <c r="Q156" s="1"/>
@@ -8314,12 +8314,12 @@
       <c r="F157" s="2"/>
       <c r="G157" s="2"/>
       <c r="H157" s="1"/>
-      <c r="I157" s="10"/>
+      <c r="I157" s="9"/>
       <c r="J157" s="1"/>
       <c r="K157" s="8"/>
       <c r="L157" s="1"/>
       <c r="M157" s="1"/>
-      <c r="N157" s="7"/>
+      <c r="N157" s="10"/>
       <c r="O157" s="1"/>
       <c r="P157" s="8"/>
       <c r="Q157" s="1"/>
@@ -8338,12 +8338,12 @@
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
       <c r="H158" s="1"/>
-      <c r="I158" s="10"/>
+      <c r="I158" s="9"/>
       <c r="J158" s="1"/>
       <c r="K158" s="8"/>
       <c r="L158" s="1"/>
       <c r="M158" s="1"/>
-      <c r="N158" s="7"/>
+      <c r="N158" s="10"/>
       <c r="O158" s="1"/>
       <c r="P158" s="8"/>
       <c r="Q158" s="1"/>
@@ -8362,12 +8362,12 @@
       <c r="F159" s="2"/>
       <c r="G159" s="2"/>
       <c r="H159" s="1"/>
-      <c r="I159" s="10"/>
+      <c r="I159" s="9"/>
       <c r="J159" s="1"/>
       <c r="K159" s="8"/>
       <c r="L159" s="1"/>
       <c r="M159" s="1"/>
-      <c r="N159" s="7"/>
+      <c r="N159" s="10"/>
       <c r="O159" s="1"/>
       <c r="P159" s="8"/>
       <c r="Q159" s="1"/>
@@ -8386,12 +8386,12 @@
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
       <c r="H160" s="1"/>
-      <c r="I160" s="10"/>
+      <c r="I160" s="9"/>
       <c r="J160" s="1"/>
       <c r="K160" s="8"/>
       <c r="L160" s="1"/>
       <c r="M160" s="1"/>
-      <c r="N160" s="7"/>
+      <c r="N160" s="10"/>
       <c r="O160" s="1"/>
       <c r="P160" s="8"/>
       <c r="Q160" s="1"/>
@@ -8410,12 +8410,12 @@
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
       <c r="H161" s="1"/>
-      <c r="I161" s="10"/>
+      <c r="I161" s="9"/>
       <c r="J161" s="1"/>
       <c r="K161" s="8"/>
       <c r="L161" s="1"/>
       <c r="M161" s="1"/>
-      <c r="N161" s="7"/>
+      <c r="N161" s="10"/>
       <c r="O161" s="1"/>
       <c r="P161" s="8"/>
       <c r="Q161" s="1"/>
@@ -8434,12 +8434,12 @@
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
       <c r="H162" s="1"/>
-      <c r="I162" s="10"/>
+      <c r="I162" s="9"/>
       <c r="J162" s="1"/>
       <c r="K162" s="8"/>
       <c r="L162" s="1"/>
       <c r="M162" s="1"/>
-      <c r="N162" s="7"/>
+      <c r="N162" s="10"/>
       <c r="O162" s="1"/>
       <c r="P162" s="8"/>
       <c r="Q162" s="1"/>
@@ -8458,12 +8458,12 @@
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
       <c r="H163" s="1"/>
-      <c r="I163" s="10"/>
+      <c r="I163" s="9"/>
       <c r="J163" s="1"/>
       <c r="K163" s="8"/>
       <c r="L163" s="1"/>
       <c r="M163" s="1"/>
-      <c r="N163" s="7"/>
+      <c r="N163" s="10"/>
       <c r="O163" s="1"/>
       <c r="P163" s="8"/>
       <c r="Q163" s="1"/>
@@ -8482,12 +8482,12 @@
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
       <c r="H164" s="1"/>
-      <c r="I164" s="10"/>
+      <c r="I164" s="9"/>
       <c r="J164" s="1"/>
       <c r="K164" s="8"/>
       <c r="L164" s="1"/>
       <c r="M164" s="1"/>
-      <c r="N164" s="7"/>
+      <c r="N164" s="10"/>
       <c r="O164" s="1"/>
       <c r="P164" s="8"/>
       <c r="Q164" s="1"/>
@@ -8506,12 +8506,12 @@
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
       <c r="H165" s="1"/>
-      <c r="I165" s="10"/>
+      <c r="I165" s="9"/>
       <c r="J165" s="1"/>
       <c r="K165" s="8"/>
       <c r="L165" s="1"/>
       <c r="M165" s="1"/>
-      <c r="N165" s="7"/>
+      <c r="N165" s="10"/>
       <c r="O165" s="1"/>
       <c r="P165" s="8"/>
       <c r="Q165" s="1"/>
@@ -8530,12 +8530,12 @@
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
       <c r="H166" s="1"/>
-      <c r="I166" s="10"/>
+      <c r="I166" s="9"/>
       <c r="J166" s="1"/>
       <c r="K166" s="8"/>
       <c r="L166" s="1"/>
       <c r="M166" s="1"/>
-      <c r="N166" s="7"/>
+      <c r="N166" s="10"/>
       <c r="O166" s="1"/>
       <c r="P166" s="8"/>
       <c r="Q166" s="1"/>
@@ -8554,12 +8554,12 @@
       <c r="F167" s="2"/>
       <c r="G167" s="2"/>
       <c r="H167" s="1"/>
-      <c r="I167" s="10"/>
+      <c r="I167" s="9"/>
       <c r="J167" s="1"/>
       <c r="K167" s="8"/>
       <c r="L167" s="1"/>
       <c r="M167" s="1"/>
-      <c r="N167" s="7"/>
+      <c r="N167" s="10"/>
       <c r="O167" s="1"/>
       <c r="P167" s="8"/>
       <c r="Q167" s="1"/>
@@ -8578,12 +8578,12 @@
       <c r="F168" s="2"/>
       <c r="G168" s="2"/>
       <c r="H168" s="1"/>
-      <c r="I168" s="10"/>
+      <c r="I168" s="9"/>
       <c r="J168" s="1"/>
       <c r="K168" s="8"/>
       <c r="L168" s="1"/>
       <c r="M168" s="1"/>
-      <c r="N168" s="7"/>
+      <c r="N168" s="10"/>
       <c r="O168" s="1"/>
       <c r="P168" s="8"/>
       <c r="Q168" s="1"/>
@@ -8602,12 +8602,12 @@
       <c r="F169" s="2"/>
       <c r="G169" s="2"/>
       <c r="H169" s="1"/>
-      <c r="I169" s="10"/>
+      <c r="I169" s="9"/>
       <c r="J169" s="1"/>
       <c r="K169" s="8"/>
       <c r="L169" s="1"/>
       <c r="M169" s="1"/>
-      <c r="N169" s="7"/>
+      <c r="N169" s="10"/>
       <c r="O169" s="1"/>
       <c r="P169" s="8"/>
       <c r="Q169" s="1"/>
@@ -8626,12 +8626,12 @@
       <c r="F170" s="2"/>
       <c r="G170" s="2"/>
       <c r="H170" s="1"/>
-      <c r="I170" s="10"/>
+      <c r="I170" s="9"/>
       <c r="J170" s="1"/>
       <c r="K170" s="8"/>
       <c r="L170" s="1"/>
       <c r="M170" s="1"/>
-      <c r="N170" s="7"/>
+      <c r="N170" s="10"/>
       <c r="O170" s="1"/>
       <c r="P170" s="8"/>
       <c r="Q170" s="1"/>
@@ -8650,12 +8650,12 @@
       <c r="F171" s="2"/>
       <c r="G171" s="2"/>
       <c r="H171" s="1"/>
-      <c r="I171" s="10"/>
+      <c r="I171" s="9"/>
       <c r="J171" s="1"/>
       <c r="K171" s="8"/>
       <c r="L171" s="1"/>
       <c r="M171" s="1"/>
-      <c r="N171" s="7"/>
+      <c r="N171" s="10"/>
       <c r="O171" s="1"/>
       <c r="P171" s="8"/>
       <c r="Q171" s="1"/>
@@ -8674,12 +8674,12 @@
       <c r="F172" s="2"/>
       <c r="G172" s="2"/>
       <c r="H172" s="1"/>
-      <c r="I172" s="10"/>
+      <c r="I172" s="9"/>
       <c r="J172" s="1"/>
       <c r="K172" s="8"/>
       <c r="L172" s="1"/>
       <c r="M172" s="1"/>
-      <c r="N172" s="7"/>
+      <c r="N172" s="10"/>
       <c r="O172" s="1"/>
       <c r="P172" s="8"/>
       <c r="Q172" s="1"/>
@@ -8698,12 +8698,12 @@
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
       <c r="H173" s="1"/>
-      <c r="I173" s="10"/>
+      <c r="I173" s="9"/>
       <c r="J173" s="1"/>
       <c r="K173" s="8"/>
       <c r="L173" s="1"/>
       <c r="M173" s="1"/>
-      <c r="N173" s="7"/>
+      <c r="N173" s="10"/>
       <c r="O173" s="1"/>
       <c r="P173" s="8"/>
       <c r="Q173" s="1"/>
@@ -8722,12 +8722,12 @@
       <c r="F174" s="2"/>
       <c r="G174" s="2"/>
       <c r="H174" s="1"/>
-      <c r="I174" s="10"/>
+      <c r="I174" s="9"/>
       <c r="J174" s="1"/>
       <c r="K174" s="8"/>
       <c r="L174" s="1"/>
       <c r="M174" s="1"/>
-      <c r="N174" s="7"/>
+      <c r="N174" s="10"/>
       <c r="O174" s="1"/>
       <c r="P174" s="8"/>
       <c r="Q174" s="1"/>
@@ -8746,12 +8746,12 @@
       <c r="F175" s="2"/>
       <c r="G175" s="2"/>
       <c r="H175" s="1"/>
-      <c r="I175" s="10"/>
+      <c r="I175" s="9"/>
       <c r="J175" s="1"/>
       <c r="K175" s="8"/>
       <c r="L175" s="1"/>
       <c r="M175" s="1"/>
-      <c r="N175" s="7"/>
+      <c r="N175" s="10"/>
       <c r="O175" s="1"/>
       <c r="P175" s="8"/>
       <c r="Q175" s="1"/>
@@ -8770,12 +8770,12 @@
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
       <c r="H176" s="1"/>
-      <c r="I176" s="10"/>
+      <c r="I176" s="9"/>
       <c r="J176" s="1"/>
       <c r="K176" s="8"/>
       <c r="L176" s="1"/>
       <c r="M176" s="1"/>
-      <c r="N176" s="7"/>
+      <c r="N176" s="10"/>
       <c r="O176" s="1"/>
       <c r="P176" s="8"/>
       <c r="Q176" s="1"/>
@@ -8794,12 +8794,12 @@
       <c r="F177" s="2"/>
       <c r="G177" s="2"/>
       <c r="H177" s="1"/>
-      <c r="I177" s="10"/>
+      <c r="I177" s="9"/>
       <c r="J177" s="1"/>
       <c r="K177" s="8"/>
       <c r="L177" s="1"/>
       <c r="M177" s="1"/>
-      <c r="N177" s="7"/>
+      <c r="N177" s="10"/>
       <c r="O177" s="1"/>
       <c r="P177" s="8"/>
       <c r="Q177" s="1"/>
@@ -8818,12 +8818,12 @@
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
       <c r="H178" s="1"/>
-      <c r="I178" s="10"/>
+      <c r="I178" s="9"/>
       <c r="J178" s="1"/>
       <c r="K178" s="8"/>
       <c r="L178" s="1"/>
       <c r="M178" s="1"/>
-      <c r="N178" s="7"/>
+      <c r="N178" s="10"/>
       <c r="O178" s="1"/>
       <c r="P178" s="8"/>
       <c r="Q178" s="1"/>
@@ -8842,12 +8842,12 @@
       <c r="F179" s="2"/>
       <c r="G179" s="2"/>
       <c r="H179" s="1"/>
-      <c r="I179" s="10"/>
+      <c r="I179" s="9"/>
       <c r="J179" s="1"/>
       <c r="K179" s="8"/>
       <c r="L179" s="1"/>
       <c r="M179" s="1"/>
-      <c r="N179" s="7"/>
+      <c r="N179" s="10"/>
       <c r="O179" s="1"/>
       <c r="P179" s="8"/>
       <c r="Q179" s="1"/>
@@ -8866,12 +8866,12 @@
       <c r="F180" s="2"/>
       <c r="G180" s="2"/>
       <c r="H180" s="1"/>
-      <c r="I180" s="10"/>
+      <c r="I180" s="9"/>
       <c r="J180" s="1"/>
       <c r="K180" s="8"/>
       <c r="L180" s="1"/>
       <c r="M180" s="1"/>
-      <c r="N180" s="7"/>
+      <c r="N180" s="10"/>
       <c r="O180" s="1"/>
       <c r="P180" s="8"/>
       <c r="Q180" s="1"/>
@@ -8890,12 +8890,12 @@
       <c r="F181" s="2"/>
       <c r="G181" s="2"/>
       <c r="H181" s="1"/>
-      <c r="I181" s="10"/>
+      <c r="I181" s="9"/>
       <c r="J181" s="1"/>
       <c r="K181" s="8"/>
       <c r="L181" s="1"/>
       <c r="M181" s="1"/>
-      <c r="N181" s="7"/>
+      <c r="N181" s="10"/>
       <c r="O181" s="1"/>
       <c r="P181" s="8"/>
       <c r="Q181" s="1"/>
@@ -8914,12 +8914,12 @@
       <c r="F182" s="2"/>
       <c r="G182" s="2"/>
       <c r="H182" s="1"/>
-      <c r="I182" s="10"/>
+      <c r="I182" s="9"/>
       <c r="J182" s="1"/>
       <c r="K182" s="8"/>
       <c r="L182" s="1"/>
       <c r="M182" s="1"/>
-      <c r="N182" s="7"/>
+      <c r="N182" s="10"/>
       <c r="O182" s="1"/>
       <c r="P182" s="8"/>
       <c r="Q182" s="1"/>
@@ -8938,12 +8938,12 @@
       <c r="F183" s="2"/>
       <c r="G183" s="2"/>
       <c r="H183" s="1"/>
-      <c r="I183" s="10"/>
+      <c r="I183" s="9"/>
       <c r="J183" s="1"/>
       <c r="K183" s="8"/>
       <c r="L183" s="1"/>
       <c r="M183" s="1"/>
-      <c r="N183" s="7"/>
+      <c r="N183" s="10"/>
       <c r="O183" s="1"/>
       <c r="P183" s="8"/>
       <c r="Q183" s="1"/>
@@ -8962,12 +8962,12 @@
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
       <c r="H184" s="1"/>
-      <c r="I184" s="10"/>
+      <c r="I184" s="9"/>
       <c r="J184" s="1"/>
       <c r="K184" s="8"/>
       <c r="L184" s="1"/>
       <c r="M184" s="1"/>
-      <c r="N184" s="7"/>
+      <c r="N184" s="10"/>
       <c r="O184" s="1"/>
       <c r="P184" s="8"/>
       <c r="Q184" s="1"/>
@@ -8986,12 +8986,12 @@
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
       <c r="H185" s="1"/>
-      <c r="I185" s="10"/>
+      <c r="I185" s="9"/>
       <c r="J185" s="1"/>
       <c r="K185" s="8"/>
       <c r="L185" s="1"/>
       <c r="M185" s="1"/>
-      <c r="N185" s="7"/>
+      <c r="N185" s="10"/>
       <c r="O185" s="1"/>
       <c r="P185" s="8"/>
       <c r="Q185" s="1"/>
@@ -9010,12 +9010,12 @@
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
       <c r="H186" s="1"/>
-      <c r="I186" s="10"/>
+      <c r="I186" s="9"/>
       <c r="J186" s="1"/>
       <c r="K186" s="8"/>
       <c r="L186" s="1"/>
       <c r="M186" s="1"/>
-      <c r="N186" s="7"/>
+      <c r="N186" s="10"/>
       <c r="O186" s="1"/>
       <c r="P186" s="8"/>
       <c r="Q186" s="1"/>
@@ -9034,12 +9034,12 @@
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
       <c r="H187" s="1"/>
-      <c r="I187" s="10"/>
+      <c r="I187" s="9"/>
       <c r="J187" s="1"/>
       <c r="K187" s="8"/>
       <c r="L187" s="1"/>
       <c r="M187" s="1"/>
-      <c r="N187" s="7"/>
+      <c r="N187" s="10"/>
       <c r="O187" s="1"/>
       <c r="P187" s="8"/>
       <c r="Q187" s="1"/>
@@ -9058,12 +9058,12 @@
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
       <c r="H188" s="1"/>
-      <c r="I188" s="10"/>
+      <c r="I188" s="9"/>
       <c r="J188" s="1"/>
       <c r="K188" s="8"/>
       <c r="L188" s="1"/>
       <c r="M188" s="1"/>
-      <c r="N188" s="7"/>
+      <c r="N188" s="10"/>
       <c r="O188" s="1"/>
       <c r="P188" s="8"/>
       <c r="Q188" s="1"/>
@@ -9082,12 +9082,12 @@
       <c r="F189" s="2"/>
       <c r="G189" s="2"/>
       <c r="H189" s="1"/>
-      <c r="I189" s="10"/>
+      <c r="I189" s="9"/>
       <c r="J189" s="1"/>
       <c r="K189" s="8"/>
       <c r="L189" s="1"/>
       <c r="M189" s="1"/>
-      <c r="N189" s="7"/>
+      <c r="N189" s="10"/>
       <c r="O189" s="1"/>
       <c r="P189" s="8"/>
       <c r="Q189" s="1"/>
@@ -9106,12 +9106,12 @@
       <c r="F190" s="2"/>
       <c r="G190" s="2"/>
       <c r="H190" s="1"/>
-      <c r="I190" s="10"/>
+      <c r="I190" s="9"/>
       <c r="J190" s="1"/>
       <c r="K190" s="8"/>
       <c r="L190" s="1"/>
       <c r="M190" s="1"/>
-      <c r="N190" s="7"/>
+      <c r="N190" s="10"/>
       <c r="O190" s="1"/>
       <c r="P190" s="8"/>
       <c r="Q190" s="1"/>
@@ -9130,12 +9130,12 @@
       <c r="F191" s="2"/>
       <c r="G191" s="2"/>
       <c r="H191" s="1"/>
-      <c r="I191" s="10"/>
+      <c r="I191" s="9"/>
       <c r="J191" s="1"/>
       <c r="K191" s="8"/>
       <c r="L191" s="1"/>
       <c r="M191" s="1"/>
-      <c r="N191" s="7"/>
+      <c r="N191" s="10"/>
       <c r="O191" s="1"/>
       <c r="P191" s="8"/>
       <c r="Q191" s="1"/>
@@ -9154,12 +9154,12 @@
       <c r="F192" s="2"/>
       <c r="G192" s="2"/>
       <c r="H192" s="1"/>
-      <c r="I192" s="10"/>
+      <c r="I192" s="9"/>
       <c r="J192" s="1"/>
       <c r="K192" s="8"/>
       <c r="L192" s="1"/>
       <c r="M192" s="1"/>
-      <c r="N192" s="7"/>
+      <c r="N192" s="10"/>
       <c r="O192" s="1"/>
       <c r="P192" s="8"/>
       <c r="Q192" s="1"/>
@@ -9178,12 +9178,12 @@
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
       <c r="H193" s="1"/>
-      <c r="I193" s="10"/>
+      <c r="I193" s="9"/>
       <c r="J193" s="1"/>
       <c r="K193" s="8"/>
       <c r="L193" s="1"/>
       <c r="M193" s="1"/>
-      <c r="N193" s="7"/>
+      <c r="N193" s="10"/>
       <c r="O193" s="1"/>
       <c r="P193" s="8"/>
       <c r="Q193" s="1"/>
@@ -9202,12 +9202,12 @@
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
       <c r="H194" s="1"/>
-      <c r="I194" s="10"/>
+      <c r="I194" s="9"/>
       <c r="J194" s="1"/>
       <c r="K194" s="8"/>
       <c r="L194" s="1"/>
       <c r="M194" s="1"/>
-      <c r="N194" s="7"/>
+      <c r="N194" s="10"/>
       <c r="O194" s="1"/>
       <c r="P194" s="8"/>
       <c r="Q194" s="1"/>
@@ -9226,12 +9226,12 @@
       <c r="F195" s="2"/>
       <c r="G195" s="2"/>
       <c r="H195" s="1"/>
-      <c r="I195" s="10"/>
+      <c r="I195" s="9"/>
       <c r="J195" s="1"/>
       <c r="K195" s="8"/>
       <c r="L195" s="1"/>
       <c r="M195" s="1"/>
-      <c r="N195" s="7"/>
+      <c r="N195" s="10"/>
       <c r="O195" s="1"/>
       <c r="P195" s="8"/>
       <c r="Q195" s="1"/>
@@ -9250,12 +9250,12 @@
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
       <c r="H196" s="1"/>
-      <c r="I196" s="10"/>
+      <c r="I196" s="9"/>
       <c r="J196" s="1"/>
       <c r="K196" s="8"/>
       <c r="L196" s="1"/>
       <c r="M196" s="1"/>
-      <c r="N196" s="7"/>
+      <c r="N196" s="10"/>
       <c r="O196" s="1"/>
       <c r="P196" s="8"/>
       <c r="Q196" s="1"/>
@@ -9274,12 +9274,12 @@
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
       <c r="H197" s="1"/>
-      <c r="I197" s="10"/>
+      <c r="I197" s="9"/>
       <c r="J197" s="1"/>
       <c r="K197" s="8"/>
       <c r="L197" s="1"/>
       <c r="M197" s="1"/>
-      <c r="N197" s="7"/>
+      <c r="N197" s="10"/>
       <c r="O197" s="1"/>
       <c r="P197" s="8"/>
       <c r="Q197" s="1"/>
@@ -9298,12 +9298,12 @@
       <c r="F198" s="2"/>
       <c r="G198" s="2"/>
       <c r="H198" s="1"/>
-      <c r="I198" s="10"/>
+      <c r="I198" s="9"/>
       <c r="J198" s="1"/>
       <c r="K198" s="8"/>
       <c r="L198" s="1"/>
       <c r="M198" s="1"/>
-      <c r="N198" s="7"/>
+      <c r="N198" s="10"/>
       <c r="O198" s="1"/>
       <c r="P198" s="8"/>
       <c r="Q198" s="1"/>
@@ -9322,12 +9322,12 @@
       <c r="F199" s="2"/>
       <c r="G199" s="2"/>
       <c r="H199" s="1"/>
-      <c r="I199" s="10"/>
+      <c r="I199" s="9"/>
       <c r="J199" s="1"/>
       <c r="K199" s="8"/>
       <c r="L199" s="1"/>
       <c r="M199" s="1"/>
-      <c r="N199" s="7"/>
+      <c r="N199" s="10"/>
       <c r="O199" s="1"/>
       <c r="P199" s="8"/>
       <c r="Q199" s="1"/>
@@ -9346,12 +9346,12 @@
       <c r="F200" s="2"/>
       <c r="G200" s="2"/>
       <c r="H200" s="1"/>
-      <c r="I200" s="10"/>
+      <c r="I200" s="9"/>
       <c r="J200" s="1"/>
       <c r="K200" s="8"/>
       <c r="L200" s="1"/>
       <c r="M200" s="1"/>
-      <c r="N200" s="7"/>
+      <c r="N200" s="10"/>
       <c r="O200" s="1"/>
       <c r="P200" s="8"/>
       <c r="Q200" s="1"/>
@@ -9370,12 +9370,12 @@
       <c r="F201" s="2"/>
       <c r="G201" s="2"/>
       <c r="H201" s="1"/>
-      <c r="I201" s="10"/>
+      <c r="I201" s="9"/>
       <c r="J201" s="1"/>
       <c r="K201" s="8"/>
       <c r="L201" s="1"/>
       <c r="M201" s="1"/>
-      <c r="N201" s="7"/>
+      <c r="N201" s="10"/>
       <c r="O201" s="1"/>
       <c r="P201" s="8"/>
       <c r="Q201" s="1"/>
@@ -9394,12 +9394,12 @@
       <c r="F202" s="2"/>
       <c r="G202" s="2"/>
       <c r="H202" s="1"/>
-      <c r="I202" s="10"/>
+      <c r="I202" s="9"/>
       <c r="J202" s="1"/>
       <c r="K202" s="8"/>
       <c r="L202" s="1"/>
       <c r="M202" s="1"/>
-      <c r="N202" s="7"/>
+      <c r="N202" s="10"/>
       <c r="O202" s="1"/>
       <c r="P202" s="8"/>
       <c r="Q202" s="1"/>
@@ -9418,12 +9418,12 @@
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>
       <c r="H203" s="1"/>
-      <c r="I203" s="10"/>
+      <c r="I203" s="9"/>
       <c r="J203" s="1"/>
       <c r="K203" s="8"/>
       <c r="L203" s="1"/>
       <c r="M203" s="1"/>
-      <c r="N203" s="7"/>
+      <c r="N203" s="10"/>
       <c r="O203" s="1"/>
       <c r="P203" s="8"/>
       <c r="Q203" s="1"/>
@@ -9442,12 +9442,12 @@
       <c r="F204" s="2"/>
       <c r="G204" s="2"/>
       <c r="H204" s="1"/>
-      <c r="I204" s="10"/>
+      <c r="I204" s="9"/>
       <c r="J204" s="1"/>
       <c r="K204" s="8"/>
       <c r="L204" s="1"/>
       <c r="M204" s="1"/>
-      <c r="N204" s="7"/>
+      <c r="N204" s="10"/>
       <c r="O204" s="1"/>
       <c r="P204" s="8"/>
       <c r="Q204" s="1"/>
@@ -9466,12 +9466,12 @@
       <c r="F205" s="2"/>
       <c r="G205" s="2"/>
       <c r="H205" s="1"/>
-      <c r="I205" s="10"/>
+      <c r="I205" s="9"/>
       <c r="J205" s="1"/>
       <c r="K205" s="8"/>
       <c r="L205" s="1"/>
       <c r="M205" s="1"/>
-      <c r="N205" s="7"/>
+      <c r="N205" s="10"/>
       <c r="O205" s="1"/>
       <c r="P205" s="8"/>
       <c r="Q205" s="1"/>
@@ -9490,12 +9490,12 @@
       <c r="F206" s="2"/>
       <c r="G206" s="2"/>
       <c r="H206" s="1"/>
-      <c r="I206" s="10"/>
+      <c r="I206" s="9"/>
       <c r="J206" s="1"/>
       <c r="K206" s="8"/>
       <c r="L206" s="1"/>
       <c r="M206" s="1"/>
-      <c r="N206" s="7"/>
+      <c r="N206" s="10"/>
       <c r="O206" s="1"/>
       <c r="P206" s="8"/>
       <c r="Q206" s="1"/>
@@ -9514,12 +9514,12 @@
       <c r="F207" s="2"/>
       <c r="G207" s="2"/>
       <c r="H207" s="1"/>
-      <c r="I207" s="10"/>
+      <c r="I207" s="9"/>
       <c r="J207" s="1"/>
       <c r="K207" s="8"/>
       <c r="L207" s="1"/>
       <c r="M207" s="1"/>
-      <c r="N207" s="7"/>
+      <c r="N207" s="10"/>
       <c r="O207" s="1"/>
       <c r="P207" s="8"/>
       <c r="Q207" s="1"/>
@@ -9538,12 +9538,12 @@
       <c r="F208" s="8"/>
       <c r="G208" s="8"/>
       <c r="H208" s="1"/>
-      <c r="I208" s="10"/>
+      <c r="I208" s="9"/>
       <c r="J208" s="1"/>
       <c r="K208" s="8"/>
       <c r="L208" s="3"/>
       <c r="M208" s="1"/>
-      <c r="N208" s="7"/>
+      <c r="N208" s="10"/>
       <c r="O208" s="1"/>
       <c r="P208" s="8"/>
       <c r="Q208" s="1"/>
@@ -9562,12 +9562,12 @@
       <c r="F209" s="8"/>
       <c r="G209" s="8"/>
       <c r="H209" s="1"/>
-      <c r="I209" s="10"/>
+      <c r="I209" s="9"/>
       <c r="J209" s="1"/>
       <c r="K209" s="8"/>
       <c r="L209" s="3"/>
       <c r="M209" s="1"/>
-      <c r="N209" s="7"/>
+      <c r="N209" s="10"/>
       <c r="O209" s="1"/>
       <c r="P209" s="8"/>
       <c r="Q209" s="1"/>
@@ -9586,12 +9586,12 @@
       <c r="F210" s="8"/>
       <c r="G210" s="8"/>
       <c r="H210" s="1"/>
-      <c r="I210" s="10"/>
+      <c r="I210" s="9"/>
       <c r="J210" s="1"/>
       <c r="K210" s="8"/>
       <c r="L210" s="3"/>
       <c r="M210" s="1"/>
-      <c r="N210" s="7"/>
+      <c r="N210" s="10"/>
       <c r="O210" s="1"/>
       <c r="P210" s="8"/>
       <c r="Q210" s="1"/>
@@ -9610,12 +9610,12 @@
       <c r="F211" s="8"/>
       <c r="G211" s="8"/>
       <c r="H211" s="1"/>
-      <c r="I211" s="10"/>
+      <c r="I211" s="9"/>
       <c r="J211" s="1"/>
       <c r="K211" s="8"/>
       <c r="L211" s="3"/>
       <c r="M211" s="1"/>
-      <c r="N211" s="7"/>
+      <c r="N211" s="10"/>
       <c r="O211" s="1"/>
       <c r="P211" s="8"/>
       <c r="Q211" s="1"/>
@@ -9634,12 +9634,12 @@
       <c r="F212" s="8"/>
       <c r="G212" s="8"/>
       <c r="H212" s="1"/>
-      <c r="I212" s="10"/>
+      <c r="I212" s="9"/>
       <c r="J212" s="1"/>
       <c r="K212" s="8"/>
       <c r="L212" s="3"/>
       <c r="M212" s="1"/>
-      <c r="N212" s="7"/>
+      <c r="N212" s="10"/>
       <c r="O212" s="1"/>
       <c r="P212" s="8"/>
       <c r="Q212" s="1"/>
@@ -9658,12 +9658,12 @@
       <c r="F213" s="8"/>
       <c r="G213" s="8"/>
       <c r="H213" s="1"/>
-      <c r="I213" s="10"/>
+      <c r="I213" s="9"/>
       <c r="J213" s="1"/>
       <c r="K213" s="8"/>
       <c r="L213" s="3"/>
       <c r="M213" s="1"/>
-      <c r="N213" s="7"/>
+      <c r="N213" s="10"/>
       <c r="O213" s="1"/>
       <c r="P213" s="8"/>
       <c r="Q213" s="1"/>
@@ -9682,12 +9682,12 @@
       <c r="F214" s="8"/>
       <c r="G214" s="8"/>
       <c r="H214" s="1"/>
-      <c r="I214" s="10"/>
+      <c r="I214" s="9"/>
       <c r="J214" s="1"/>
       <c r="K214" s="8"/>
       <c r="L214" s="3"/>
       <c r="M214" s="1"/>
-      <c r="N214" s="7"/>
+      <c r="N214" s="10"/>
       <c r="O214" s="1"/>
       <c r="P214" s="8"/>
       <c r="Q214" s="1"/>
@@ -9706,12 +9706,12 @@
       <c r="F215" s="8"/>
       <c r="G215" s="8"/>
       <c r="H215" s="1"/>
-      <c r="I215" s="10"/>
+      <c r="I215" s="9"/>
       <c r="J215" s="1"/>
       <c r="K215" s="8"/>
       <c r="L215" s="3"/>
       <c r="M215" s="1"/>
-      <c r="N215" s="7"/>
+      <c r="N215" s="10"/>
       <c r="O215" s="1"/>
       <c r="P215" s="8"/>
       <c r="Q215" s="1"/>

</xml_diff>